<commit_message>
real feed memes added
</commit_message>
<xml_diff>
--- a/_static/global/HR.xlsx
+++ b/_static/global/HR.xlsx
@@ -94,8 +94,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -113,11 +117,15 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -450,7 +458,7 @@
   <dimension ref="A1:H109"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -511,10 +519,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="3">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C5" s="3">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -698,10 +706,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="3">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C22" s="3">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1175,28 +1183,6 @@
       </c>
       <c r="C65" s="3">
         <v>10</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="3">
-        <v>65</v>
-      </c>
-      <c r="B66" s="3">
-        <v>29</v>
-      </c>
-      <c r="C66" s="3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="3">
-        <v>66</v>
-      </c>
-      <c r="B67" s="3">
-        <v>34</v>
-      </c>
-      <c r="C67" s="3">
-        <v>6</v>
       </c>
     </row>
     <row r="70" spans="1:3">

</xml_diff>